<commit_message>
Code for the cleaning process and visualization is added with its output
</commit_message>
<xml_diff>
--- a/DataCleaninig/Data.xlsx
+++ b/DataCleaninig/Data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
   <si>
     <t>S.N.</t>
   </si>
@@ -94,6 +94,18 @@
   </si>
   <si>
     <t>Kabre</t>
+  </si>
+  <si>
+    <t>Sailesh Shapkota</t>
+  </si>
+  <si>
+    <t>Pratik Chaudhary</t>
+  </si>
+  <si>
+    <t>Twenty</t>
+  </si>
+  <si>
+    <t>Kapilbastu</t>
   </si>
 </sst>
 </file>
@@ -144,9 +156,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -648,6 +661,96 @@
         <v>22</v>
       </c>
     </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2">
+        <v>23</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="2">
+        <v>3.8</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1">
+        <v>22</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="1">
+        <v>3.9</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>